<commit_message>
Compte de résultat en tableau _ Systeme de base
</commit_message>
<xml_diff>
--- a/France/3_Comptabilite_Et_Fiscalite/2_Compte_De_Resultat/Compte_De_Resultat.xlsx
+++ b/France/3_Comptabilite_Et_Fiscalite/2_Compte_De_Resultat/Compte_De_Resultat.xlsx
@@ -11,24 +11,247 @@
     <sheet name="Systeme_Abrege" sheetId="2" r:id="rId2"/>
     <sheet name="Systeme_Developpe" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="71">
   <si>
     <t xml:space="preserve"> Modèle de compte de résultat en tableau</t>
   </si>
   <si>
     <t>CHARGES (hors taxes)</t>
+  </si>
+  <si>
+    <t>Exercice N-1 [€]</t>
+  </si>
+  <si>
+    <t>Exercice N [€]</t>
+  </si>
+  <si>
+    <t>Charges d'exploitation (1) :</t>
+  </si>
+  <si>
+    <t>Achats de marchandises (a)</t>
+  </si>
+  <si>
+    <t>Variation des stocks (b)</t>
+  </si>
+  <si>
+    <t>Achats de matières premières et autres approvisionnements (a)</t>
+  </si>
+  <si>
+    <t>* Autres achats et charges externes</t>
+  </si>
+  <si>
+    <t>Impôts, taxes et versements assimilés</t>
+  </si>
+  <si>
+    <t>Salaires et traitements</t>
+  </si>
+  <si>
+    <t>Charges sociales</t>
+  </si>
+  <si>
+    <t>Dotations aux amortissements et dépréciations :</t>
+  </si>
+  <si>
+    <t>Sur immobilisations : dotations aux amortissements ('c')</t>
+  </si>
+  <si>
+    <t>Sur immobilisations : dotations aux dépréciations</t>
+  </si>
+  <si>
+    <t>Sur actif circulant : dotations aux dépréciations</t>
+  </si>
+  <si>
+    <t>Dotations aux provisions</t>
+  </si>
+  <si>
+    <t>Autres charges</t>
+  </si>
+  <si>
+    <t>TOTAL (I)</t>
+  </si>
+  <si>
+    <t>Charges financières :</t>
+  </si>
+  <si>
+    <t>Dotations aux amortissements, aux dépréciations et aux provisions</t>
+  </si>
+  <si>
+    <t>Intérêts et charges assimilées (2)</t>
+  </si>
+  <si>
+    <t>Différences négatives de change</t>
+  </si>
+  <si>
+    <t>Charges nettes sur cessions de valeurs mobilières de placement</t>
+  </si>
+  <si>
+    <t>Quote-parts de résultat sur opérations faites en commun (II)</t>
+  </si>
+  <si>
+    <t>TOTAL (III)</t>
+  </si>
+  <si>
+    <t>Charges exceptionnelles :</t>
+  </si>
+  <si>
+    <t>Sur opérations de gestion</t>
+  </si>
+  <si>
+    <t>Sur opérations en capital</t>
+  </si>
+  <si>
+    <t>TOTAL (IV)</t>
+  </si>
+  <si>
+    <t>Participation des salariés aux résultats (V)</t>
+  </si>
+  <si>
+    <t>Impôts sur les bénéfices (VI)</t>
+  </si>
+  <si>
+    <t>Total des charges (I + II + III + IV + V + VI)</t>
+  </si>
+  <si>
+    <t>Solde créditeur = bénéfice (3)</t>
+  </si>
+  <si>
+    <t>TOTAL GENERAL</t>
+  </si>
+  <si>
+    <t>* Y compris
+- redevances de crédit-bail mobilier
+- redevances de crédit-bail immobilier</t>
+  </si>
+  <si>
+    <t>(1) Dont charges afférentes à des exercices antérieurs. Les conséquences des corrections
+d’erreurs significatives, calculées après impôt, sont présentées sur une ligne séparée sauf s’il
+s’agit de corriger une écriture ayant été directement imputée sur les capitaux propres.</t>
+  </si>
+  <si>
+    <t>(2) Dont intérêts concernant les entités liées</t>
+  </si>
+  <si>
+    <t>(3) Compte tenu d'un résultat exceptionnel avant impôts de</t>
+  </si>
+  <si>
+    <t>(a) Y compris droits de douane.</t>
+  </si>
+  <si>
+    <t>(b) Stock initial moins stock final : montant de la variation en moins entre parenthèse ou précédé du signe (-).</t>
+  </si>
+  <si>
+    <t>(c) Y compris éventuellement dotations aux amortissements des charges à répartir.</t>
+  </si>
+  <si>
+    <t>PRODUITS (hors taxes)</t>
+  </si>
+  <si>
+    <t>Produits d'exploitation (1) :</t>
+  </si>
+  <si>
+    <t>Ventes de marchandises</t>
+  </si>
+  <si>
+    <t>Production vendue [biens et services] (a)</t>
+  </si>
+  <si>
+    <t>Sous total A - Montant net du chiffre d'affaires</t>
+  </si>
+  <si>
+    <t>Production stockée (b)</t>
+  </si>
+  <si>
+    <t>Production immobilisée</t>
+  </si>
+  <si>
+    <t>Subventions d'exploitation</t>
+  </si>
+  <si>
+    <t>Reprises sur provisions, dépréciations (et amortissements) et transferts de charges</t>
+  </si>
+  <si>
+    <t>Autres produits</t>
+  </si>
+  <si>
+    <t>Sous total B</t>
+  </si>
+  <si>
+    <t>Total I (A + B )</t>
+  </si>
+  <si>
+    <t>Montant net du chiffre d'affaires dont à l'exportation :</t>
+  </si>
+  <si>
+    <t>Quote-part de résultat sur opérations faites en commun (II)</t>
+  </si>
+  <si>
+    <t>Produits financiers :</t>
+  </si>
+  <si>
+    <t>De participation (2)</t>
+  </si>
+  <si>
+    <t>D'autres valeurs mobilières et créances de l'actif immobilisé (2)</t>
+  </si>
+  <si>
+    <t>Autres intérêts et produits assimilés (2)</t>
+  </si>
+  <si>
+    <t>Reprises sur provisions, dépréciations et transferts de charges</t>
+  </si>
+  <si>
+    <t>Différences positives de change</t>
+  </si>
+  <si>
+    <t>Produits nets sur cessions de valeurs mobilières de placement</t>
+  </si>
+  <si>
+    <t>Total (III)</t>
+  </si>
+  <si>
+    <t>Produits exceptionnels :</t>
+  </si>
+  <si>
+    <t>Total des produits (I + II + III + IV)</t>
+  </si>
+  <si>
+    <t>Solde débiteur = perte (3)</t>
+  </si>
+  <si>
+    <t>(1) Dont produits afférents à des exercices antérieurs. Les conséquences des corrections
+d’erreurs significatives, calculées après impôt, sont présentées sur une ligne séparée sauf s’il
+s’agit de corriger une écriture ayant été directement imputée sur les capitaux propres.</t>
+  </si>
+  <si>
+    <t>(2) Dont produits concernant les entités liées.</t>
+  </si>
+  <si>
+    <t>(a) A inscrire, le cas échéant, sur des lignes distinctes.</t>
+  </si>
+  <si>
+    <t>(b) Stock final moins stock initial : montant de la variation en moins entre parenthèses ou précédé du signe (-).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -37,15 +260,57 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -53,17 +318,94 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Monétaire" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -366,28 +708,667 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:C79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="11">
+        <f>SUM(B5:B12)</f>
+        <v>0</v>
+      </c>
+      <c r="C4" s="11">
+        <f>SUM(C5:C12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+    </row>
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+    </row>
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="13">
+        <f>SUM(B14:B17)</f>
+        <v>0</v>
+      </c>
+      <c r="C13" s="13">
+        <f>SUM(C14:C17)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+    </row>
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+    </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="15">
+        <f>SUM(B18,B13,B4)</f>
+        <v>0</v>
+      </c>
+      <c r="C19" s="15">
+        <f>SUM(C18,C13,C4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="11">
+        <f>SUM(B22:B25)</f>
+        <v>0</v>
+      </c>
+      <c r="C21" s="11">
+        <f>SUM(C22:C25)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+    </row>
+    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="15">
+        <f>B21</f>
+        <v>0</v>
+      </c>
+      <c r="C26" s="15">
+        <f>C21</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+    </row>
+    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" s="19">
+        <f>SUM(B31:B33,B26,B19:B20)</f>
+        <v>0</v>
+      </c>
+      <c r="C34" s="19">
+        <f>SUM(C31:C33,C26,C19:C20)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" s="19">
+        <f>SUM(B34:B35)</f>
+        <v>0</v>
+      </c>
+      <c r="C36" s="19">
+        <f>SUM(C34:C35)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A37" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" s="16"/>
+      <c r="C37" s="16"/>
+    </row>
+    <row r="38" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A38" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" s="17"/>
+      <c r="C38" s="17"/>
+    </row>
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" s="16"/>
+      <c r="C39" s="16"/>
+    </row>
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" s="16"/>
+      <c r="C40" s="16"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+    </row>
+    <row r="42" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
+    </row>
+    <row r="43" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B46" s="11">
+        <f>SUM(B47:B48)</f>
+        <v>0</v>
+      </c>
+      <c r="C46" s="11">
+        <f>SUM(C47:C48)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B47" s="12"/>
+      <c r="C47" s="12"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B48" s="12"/>
+      <c r="C48" s="12"/>
+    </row>
+    <row r="49" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B49" s="15">
+        <f>B46</f>
+        <v>0</v>
+      </c>
+      <c r="C49" s="15">
+        <f>C46</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B50" s="15"/>
+      <c r="C50" s="15"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B52" s="11"/>
+      <c r="C52" s="11"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B53" s="11"/>
+      <c r="C53" s="11"/>
+    </row>
+    <row r="54" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B54" s="11"/>
+      <c r="C54" s="11"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B55" s="11"/>
+      <c r="C55" s="11"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B56" s="15"/>
+      <c r="C56" s="15"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B57" s="15">
+        <f>SUM(B49,B56)</f>
+        <v>0</v>
+      </c>
+      <c r="C57" s="15">
+        <f>SUM(C49,C56)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B58" s="20"/>
+      <c r="C58" s="20"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B59" s="13">
+        <f>SUM(B60:B65)</f>
+        <v>0</v>
+      </c>
+      <c r="C59" s="13">
+        <f>SUM(C60:C65)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B60" s="14"/>
+      <c r="C60" s="14"/>
+    </row>
+    <row r="61" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B61" s="14"/>
+      <c r="C61" s="14"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B62" s="14"/>
+      <c r="C62" s="14"/>
+    </row>
+    <row r="63" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B63" s="14"/>
+      <c r="C63" s="14"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B64" s="14"/>
+      <c r="C64" s="14"/>
+    </row>
+    <row r="65" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B65" s="12"/>
+      <c r="C65" s="12"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B66" s="15">
+        <f>B59</f>
+        <v>0</v>
+      </c>
+      <c r="C66" s="15">
+        <f>C59</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B67" s="11">
+        <f>SUM(B68:B70)</f>
+        <v>0</v>
+      </c>
+      <c r="C67" s="11">
+        <f>SUM(C68:C70)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B68" s="12"/>
+      <c r="C68" s="12"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B69" s="12"/>
+      <c r="C69" s="12"/>
+    </row>
+    <row r="70" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B70" s="12"/>
+      <c r="C70" s="12"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B71" s="15">
+        <f>B67</f>
+        <v>0</v>
+      </c>
+      <c r="C71" s="15">
+        <f>C67</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B72" s="15">
+        <f>SUM(B57,B58,B66,B71)</f>
+        <v>0</v>
+      </c>
+      <c r="C72" s="15">
+        <f>SUM(C57,C58,C66,C71)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B73" s="10"/>
+      <c r="C73" s="10"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B74" s="21">
+        <f>SUM(B72:B73)</f>
+        <v>0</v>
+      </c>
+      <c r="C74" s="21">
+        <f>SUM(C72:C73)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A75" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B75" s="16"/>
+      <c r="C75" s="16"/>
+    </row>
+    <row r="76" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B76" s="16"/>
+      <c r="C76" s="16"/>
+    </row>
+    <row r="77" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A77" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B77" s="16"/>
+      <c r="C77" s="16"/>
+    </row>
+    <row r="78" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A78" s="18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A79" s="18" t="s">
+        <v>70</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Compte de résultat en liste _ Systeme de base
</commit_message>
<xml_diff>
--- a/France/3_Comptabilite_Et_Fiscalite/2_Compte_De_Resultat/Compte_De_Resultat.xlsx
+++ b/France/3_Comptabilite_Et_Fiscalite/2_Compte_De_Resultat/Compte_De_Resultat.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="114">
   <si>
     <t xml:space="preserve"> Modèle de compte de résultat en tableau</t>
   </si>
@@ -235,6 +235,143 @@
   </si>
   <si>
     <t>(b) Stock final moins stock initial : montant de la variation en moins entre parenthèses ou précédé du signe (-).</t>
+  </si>
+  <si>
+    <t>Modèle de compte de résultat en liste (produits et charges hors taxes)</t>
+  </si>
+  <si>
+    <t>Montant net du chiffre d'affaires</t>
+  </si>
+  <si>
+    <t>Reprises sur provisions (et amortissements), transferts de charges</t>
+  </si>
+  <si>
+    <t>Total (I)</t>
+  </si>
+  <si>
+    <t>Charges d'exploitation (2) :</t>
+  </si>
+  <si>
+    <t>Achats de marchandises (d) :</t>
+  </si>
+  <si>
+    <t>Variation de stock ('e')</t>
+  </si>
+  <si>
+    <t>Achats de matières premières et autres approvisionnements ('c')</t>
+  </si>
+  <si>
+    <t>Variation de stock (d)</t>
+  </si>
+  <si>
+    <t>Dotations aux amortissements et aux dépréciations :</t>
+  </si>
+  <si>
+    <t>Sur immobilisations : dotations aux amortissements ('e')</t>
+  </si>
+  <si>
+    <t>Total (II)</t>
+  </si>
+  <si>
+    <t>* Y compris :
+- Redevances de crédit-bail mobilier
+- Redevances de crédit-bail immobilier</t>
+  </si>
+  <si>
+    <t>(1) Dont produits afférents à des exercices antérieurs. Les conséquences des corrections d’erreurs significatives, calculées
+après impôt, sont présentées sur une ligne séparée sauf s’il s’agit de corriger une écriture ayant été directement imputée sur
+les capitaux propres.</t>
+  </si>
+  <si>
+    <t>(2) Dont charges afférentes à des exercices antérieurs. Les conséquences des corrections d’erreurs significatives, calculées
+après impôt, sont présentées sur une ligne séparée sauf s’il s’agit de corriger une écriture ayant été directement imputée sur
+les capitaux propres.</t>
+  </si>
+  <si>
+    <t>(c) Y compris droits de douane.</t>
+  </si>
+  <si>
+    <t>(d) Stock initial moins stock final : montant de la variation en moins entre parenthèses ou précédé du signe (-).</t>
+  </si>
+  <si>
+    <t>(e) Y compris éventuellement dotations aux amortissements des charges à répartir.</t>
+  </si>
+  <si>
+    <t>1. RESULTAT D'EXPLOITATION (I -II)</t>
+  </si>
+  <si>
+    <t>Quote-part de résultat sur opérations faites en commun :</t>
+  </si>
+  <si>
+    <t>Bénéfice ou perte transférée (III)</t>
+  </si>
+  <si>
+    <t>Pertes ou bénéfice transféré (IV)</t>
+  </si>
+  <si>
+    <t>De participation (3)</t>
+  </si>
+  <si>
+    <t>D'autres valeurs mobilières et créances de l'actif immobilisé (3)</t>
+  </si>
+  <si>
+    <t>Autres intérêts et produits assimilés (3)</t>
+  </si>
+  <si>
+    <t>Reprises sur provisions, dépréciations et transferts de charge</t>
+  </si>
+  <si>
+    <t>Total (V)</t>
+  </si>
+  <si>
+    <t>Intérêts et charges assimilées (4)</t>
+  </si>
+  <si>
+    <t>Total (VI)</t>
+  </si>
+  <si>
+    <t>2. RESULTAT FINANCIER (V - VI)</t>
+  </si>
+  <si>
+    <t>3. RESULTAT COURANT avant impôts (I - II + III - IV + V - VI)</t>
+  </si>
+  <si>
+    <t>Reprises sur provisions et dépréciations et transferts de charges</t>
+  </si>
+  <si>
+    <t>Total (VII)</t>
+  </si>
+  <si>
+    <t>Total (VIII)</t>
+  </si>
+  <si>
+    <t>4. RESULTAT EXCEPTIONNEL (VII – VIII)</t>
+  </si>
+  <si>
+    <t>Participation des salariés aux résultats (IX)</t>
+  </si>
+  <si>
+    <t>Impôts sur les bénéfices (X)</t>
+  </si>
+  <si>
+    <t>Total des produits (I + III + V + VII)</t>
+  </si>
+  <si>
+    <t>Total des charges (II + IV + VI + VIII + IX + X)</t>
+  </si>
+  <si>
+    <t>Bénéfice ou perte</t>
+  </si>
+  <si>
+    <t>(3) Dont produits concernant les entités liées</t>
+  </si>
+  <si>
+    <t>(4) Dont intérêts concernant les entités liées</t>
+  </si>
+  <si>
+    <t>N.B. - Outre le résultat exceptionnel avant impôts que les sociétés de capitaux doivent faire ressortir, les entités
+ont la faculté de faire apparaître distinctement le résultat d'exploitation et le résultat financier. Le bénéfice ou la
+perte résulte alors de la somme algébrique des résultats courant et exceptionnel (3 + 4) et les charges IX et X.</t>
   </si>
 </sst>
 </file>
@@ -260,7 +397,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -305,12 +442,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -333,12 +476,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -385,23 +565,53 @@
     <xf numFmtId="44" fontId="0" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="44" fontId="0" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -708,10 +918,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C79"/>
+  <dimension ref="A1:C160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80"/>
+    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
+      <selection activeCell="C162" sqref="C162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1365,9 +1575,669 @@
         <v>70</v>
       </c>
     </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B82" s="23"/>
+      <c r="C82" s="24"/>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="2"/>
+      <c r="B84" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B85" s="13">
+        <f>SUM(B86:B87)</f>
+        <v>0</v>
+      </c>
+      <c r="C85" s="13">
+        <f>SUM(C86:C87)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B86" s="14"/>
+      <c r="C86" s="14"/>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B87" s="14"/>
+      <c r="C87" s="14"/>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B88" s="20">
+        <f>B85</f>
+        <v>0</v>
+      </c>
+      <c r="C88" s="20">
+        <f>C85</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A89" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B89" s="20"/>
+      <c r="C89" s="20"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B90" s="13"/>
+      <c r="C90" s="13"/>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B91" s="13"/>
+      <c r="C91" s="13"/>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B92" s="13"/>
+      <c r="C92" s="13"/>
+    </row>
+    <row r="93" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A93" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B93" s="13"/>
+      <c r="C93" s="13"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B94" s="13"/>
+      <c r="C94" s="13"/>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B95" s="20">
+        <f>SUM(B90:B94,B85)</f>
+        <v>0</v>
+      </c>
+      <c r="C95" s="20">
+        <f>SUM(C90:C94,C85)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B96" s="13">
+        <f>SUM(B97,B99,B101:B104)</f>
+        <v>0</v>
+      </c>
+      <c r="C96" s="13">
+        <f>SUM(C97,C99,C101:C104)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B97" s="14"/>
+      <c r="C97" s="14"/>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B98" s="27"/>
+      <c r="C98" s="27"/>
+    </row>
+    <row r="99" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A99" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B99" s="14"/>
+      <c r="C99" s="14"/>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="B100" s="27"/>
+      <c r="C100" s="27"/>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B101" s="14"/>
+      <c r="C101" s="14"/>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B102" s="14"/>
+      <c r="C102" s="14"/>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B103" s="14"/>
+      <c r="C103" s="14"/>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B104" s="14"/>
+      <c r="C104" s="14"/>
+    </row>
+    <row r="105" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A105" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B105" s="13">
+        <f>SUM(B106:B108)</f>
+        <v>0</v>
+      </c>
+      <c r="C105" s="13">
+        <f>SUM(C106:C108)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A106" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B106" s="14"/>
+      <c r="C106" s="14"/>
+    </row>
+    <row r="107" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A107" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B107" s="14"/>
+      <c r="C107" s="14"/>
+    </row>
+    <row r="108" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A108" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B108" s="14"/>
+      <c r="C108" s="14"/>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B109" s="13"/>
+      <c r="C109" s="13"/>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B110" s="13"/>
+      <c r="C110" s="13"/>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B111" s="20">
+        <f>SUM(B109:B110,B105,B96)</f>
+        <v>0</v>
+      </c>
+      <c r="C111" s="20">
+        <f>SUM(C109:C110,C105,C96)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A112" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B112" s="25"/>
+      <c r="C112" s="25"/>
+    </row>
+    <row r="113" spans="1:3" ht="87" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="B113" s="29"/>
+      <c r="C113" s="30"/>
+    </row>
+    <row r="114" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="B114" s="29"/>
+      <c r="C114" s="30"/>
+    </row>
+    <row r="115" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A115" s="18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A116" s="18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A118" s="18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A119" s="18" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="2"/>
+      <c r="B121" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B122" s="20">
+        <f>B95-B111</f>
+        <v>0</v>
+      </c>
+      <c r="C122" s="20">
+        <f>C95-C111</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A123" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B123" s="20"/>
+      <c r="C123" s="20"/>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B124" s="20"/>
+      <c r="C124" s="20"/>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B125" s="20"/>
+      <c r="C125" s="20"/>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B126" s="13">
+        <f>SUM(B127:B132)</f>
+        <v>0</v>
+      </c>
+      <c r="C126" s="13">
+        <f>SUM(C127:C132)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B127" s="14"/>
+      <c r="C127" s="14"/>
+    </row>
+    <row r="128" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A128" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B128" s="14"/>
+      <c r="C128" s="14"/>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B129" s="14"/>
+      <c r="C129" s="14"/>
+    </row>
+    <row r="130" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A130" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B130" s="14"/>
+      <c r="C130" s="14"/>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B131" s="14"/>
+      <c r="C131" s="14"/>
+    </row>
+    <row r="132" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A132" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B132" s="14"/>
+      <c r="C132" s="14"/>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B133" s="20">
+        <f>B126</f>
+        <v>0</v>
+      </c>
+      <c r="C133" s="20">
+        <f>C126</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B134" s="13">
+        <f>SUM(B135:B138)</f>
+        <v>0</v>
+      </c>
+      <c r="C134" s="13">
+        <f>SUM(C135:C138)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A135" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B135" s="14"/>
+      <c r="C135" s="14"/>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B136" s="14"/>
+      <c r="C136" s="14"/>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B137" s="14"/>
+      <c r="C137" s="14"/>
+    </row>
+    <row r="138" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A138" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B138" s="14"/>
+      <c r="C138" s="14"/>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B139" s="20">
+        <f>B134</f>
+        <v>0</v>
+      </c>
+      <c r="C139" s="20">
+        <f>C134</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B140" s="20">
+        <f>B133-B139</f>
+        <v>0</v>
+      </c>
+      <c r="C140" s="20">
+        <f>C133-C139</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A141" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B141" s="20">
+        <f>B95-B111+B124-B125+B133-B139</f>
+        <v>0</v>
+      </c>
+      <c r="C141" s="20">
+        <f>C95-C111+C124-C125+C133-C139</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B142" s="13">
+        <f>SUM(B143:B145)</f>
+        <v>0</v>
+      </c>
+      <c r="C142" s="13">
+        <f>SUM(C143:C145)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B143" s="14"/>
+      <c r="C143" s="14"/>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B144" s="14"/>
+      <c r="C144" s="14"/>
+    </row>
+    <row r="145" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A145" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B145" s="14"/>
+      <c r="C145" s="14"/>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B146" s="20">
+        <f>B142</f>
+        <v>0</v>
+      </c>
+      <c r="C146" s="20">
+        <f>C142</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B147" s="13">
+        <f>SUM(B148:B150)</f>
+        <v>0</v>
+      </c>
+      <c r="C147" s="13">
+        <f>SUM(C148:C150)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B148" s="14"/>
+      <c r="C148" s="14"/>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B149" s="14"/>
+      <c r="C149" s="14"/>
+    </row>
+    <row r="150" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A150" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B150" s="14"/>
+      <c r="C150" s="14"/>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B151" s="20">
+        <f>B147</f>
+        <v>0</v>
+      </c>
+      <c r="C151" s="20">
+        <f>C147</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B152" s="20">
+        <f>B146-B151</f>
+        <v>0</v>
+      </c>
+      <c r="C152" s="20">
+        <f>C146-C151</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A153" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B153" s="20"/>
+      <c r="C153" s="20"/>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B154" s="20"/>
+      <c r="C154" s="20"/>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B155" s="20">
+        <f>B95+B124+B133+B146</f>
+        <v>0</v>
+      </c>
+      <c r="C155" s="20">
+        <f>C95+C124+C133+C146</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B156" s="20">
+        <f>B111+B125+B139+B151+B153+B154</f>
+        <v>0</v>
+      </c>
+      <c r="C156" s="20">
+        <f>C111+C125+C139+C151+C153+C154</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B157" s="20">
+        <f>B141+B152+B153+B154</f>
+        <v>0</v>
+      </c>
+      <c r="C157" s="20">
+        <f>C141+C152+C153+C154</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A158" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="B158" s="25"/>
+      <c r="C158" s="25"/>
+    </row>
+    <row r="159" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A159" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B159" s="25"/>
+      <c r="C159" s="25"/>
+    </row>
+    <row r="160" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A160" s="31" t="s">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
     <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A82:C82"/>
+    <mergeCell ref="A113:C113"/>
+    <mergeCell ref="A114:C114"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Compte de resultat en tableau _ Système abrege
</commit_message>
<xml_diff>
--- a/France/3_Comptabilite_Et_Fiscalite/2_Compte_De_Resultat/Compte_De_Resultat.xlsx
+++ b/France/3_Comptabilite_Et_Fiscalite/2_Compte_De_Resultat/Compte_De_Resultat.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Systeme_De_Base" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="145">
   <si>
     <t xml:space="preserve"> Modèle de compte de résultat en tableau</t>
   </si>
@@ -372,6 +372,106 @@
     <t>N.B. - Outre le résultat exceptionnel avant impôts que les sociétés de capitaux doivent faire ressortir, les entités
 ont la faculté de faire apparaître distinctement le résultat d'exploitation et le résultat financier. Le bénéfice ou la
 perte résulte alors de la somme algébrique des résultats courant et exceptionnel (3 + 4) et les charges IX et X.</t>
+  </si>
+  <si>
+    <t>Modèle de compte de résultat en tableau</t>
+  </si>
+  <si>
+    <t>Charges (hors taxes)</t>
+  </si>
+  <si>
+    <t>Produits (hors taxes)</t>
+  </si>
+  <si>
+    <t>Charges d'exploitation :</t>
+  </si>
+  <si>
+    <t>Produits d'exploitation :</t>
+  </si>
+  <si>
+    <t>Variation de stocks [marchandises] (b)</t>
+  </si>
+  <si>
+    <t>Achats d'approvisionnements (a)</t>
+  </si>
+  <si>
+    <t>Variation de stocks
+[approvisionnements] (b)</t>
+  </si>
+  <si>
+    <t>* Autres charges externes</t>
+  </si>
+  <si>
+    <t>Rémunérations du personnel</t>
+  </si>
+  <si>
+    <t>Dotations aux amortissements</t>
+  </si>
+  <si>
+    <t>Dotations aux dépréciations</t>
+  </si>
+  <si>
+    <t>Charges financières</t>
+  </si>
+  <si>
+    <t>Charges exceptionnelles (II)</t>
+  </si>
+  <si>
+    <t>Impôts sur les bénéfices (III)</t>
+  </si>
+  <si>
+    <t>Total des charges (I + II + III)</t>
+  </si>
+  <si>
+    <t>Solde créditeur : bénéfice (1)</t>
+  </si>
+  <si>
+    <t>* Y compris :
+- redevances de crédit-bail mobilier
+- redevances de crédit-bail immobilier</t>
+  </si>
+  <si>
+    <t>(b) Stock initial moins stock final : montant de la variation en moins entre parenthèses ou précédé du signe (-).</t>
+  </si>
+  <si>
+    <t>(1) Compte tenu d'un résultat
+exceptionnel avant impôts de</t>
+  </si>
+  <si>
+    <t>(2) Dont reprises sur dépréciations,
+provisions (et amortissements)
+(3) Compte tenu d’un résultat
+exceptionnel avant impôts de</t>
+  </si>
+  <si>
+    <t>(c) A inscrire, le cas échéant, sur des lignes distinctes.</t>
+  </si>
+  <si>
+    <t>(d) Stock final moins stock initial : montant de la variation en moins entre parenthèses ou précédé du signe (-)</t>
+  </si>
+  <si>
+    <t>Production vendue [biens et services] ('c')</t>
+  </si>
+  <si>
+    <t>Production stockée (d)</t>
+  </si>
+  <si>
+    <t>Autres produits (2)</t>
+  </si>
+  <si>
+    <t>Produits financiers (2)</t>
+  </si>
+  <si>
+    <t>dont à l'exportation</t>
+  </si>
+  <si>
+    <t>Produits exceptionnels (2) (II)</t>
+  </si>
+  <si>
+    <t>Total des produits (I + II)</t>
+  </si>
+  <si>
+    <t>Solde débiteur : perte (3)</t>
   </si>
 </sst>
 </file>
@@ -453,7 +553,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -513,76 +613,117 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -592,15 +733,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -610,8 +742,35 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="6" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -920,8 +1079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
-      <selection activeCell="C162" sqref="C162"/>
+    <sheetView topLeftCell="A110" workbookViewId="0">
+      <selection activeCell="A111" sqref="A111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -932,1303 +1091,1303 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="A1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="10">
         <f>SUM(B5:B12)</f>
         <v>0</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="10">
         <f>SUM(C5:C12)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="13">
+      <c r="B13" s="12">
         <f>SUM(B14:B17)</f>
         <v>0</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="12">
         <f>SUM(C14:C17)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
     </row>
     <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
     </row>
     <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="15">
+      <c r="B19" s="14">
         <f>SUM(B18,B13,B4)</f>
         <v>0</v>
       </c>
-      <c r="C19" s="15">
+      <c r="C19" s="14">
         <f>SUM(C18,C13,C4)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="11">
+      <c r="B21" s="10">
         <f>SUM(B22:B25)</f>
         <v>0</v>
       </c>
-      <c r="C21" s="11">
+      <c r="C21" s="10">
         <f>SUM(C22:C25)</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
     </row>
     <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="15">
+      <c r="B26" s="14">
         <f>B21</f>
         <v>0</v>
       </c>
-      <c r="C26" s="15">
+      <c r="C26" s="14">
         <f>C21</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
     </row>
     <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
+      <c r="A32" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
+      <c r="A33" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="19">
+      <c r="B34" s="18">
         <f>SUM(B31:B33,B26,B19:B20)</f>
         <v>0</v>
       </c>
-      <c r="C34" s="19">
+      <c r="C34" s="18">
         <f>SUM(C31:C33,C26,C19:C20)</f>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
+      <c r="A35" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="9" t="s">
+      <c r="A36" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="19">
+      <c r="B36" s="18">
         <f>SUM(B34:B35)</f>
         <v>0</v>
       </c>
-      <c r="C36" s="19">
+      <c r="C36" s="18">
         <f>SUM(C34:C35)</f>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A37" s="16" t="s">
+      <c r="A37" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="16"/>
-      <c r="C37" s="16"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="15"/>
     </row>
     <row r="38" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A38" s="16" t="s">
+      <c r="A38" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B38" s="17"/>
-      <c r="C38" s="17"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="16"/>
     </row>
     <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="16" t="s">
+      <c r="A39" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B39" s="16"/>
-      <c r="C39" s="16"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="15"/>
     </row>
     <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="16" t="s">
+      <c r="A40" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="B40" s="16"/>
-      <c r="C40" s="16"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="15"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="18" t="s">
+      <c r="A41" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
     </row>
     <row r="42" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="18" t="s">
+      <c r="A42" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
     </row>
     <row r="43" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A43" s="18" t="s">
+      <c r="A43" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="B43" s="8"/>
-      <c r="C43" s="8"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
+      <c r="A45" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="7" t="s">
+      <c r="A46" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B46" s="11">
+      <c r="B46" s="10">
         <f>SUM(B47:B48)</f>
         <v>0</v>
       </c>
-      <c r="C46" s="11">
+      <c r="C46" s="10">
         <f>SUM(C47:C48)</f>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
+      <c r="A47" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B47" s="12"/>
-      <c r="C47" s="12"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
+      <c r="A48" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B48" s="12"/>
-      <c r="C48" s="12"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="11"/>
     </row>
     <row r="49" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="9" t="s">
+      <c r="A49" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B49" s="15">
+      <c r="B49" s="14">
         <f>B46</f>
         <v>0</v>
       </c>
-      <c r="C49" s="15">
+      <c r="C49" s="14">
         <f>C46</f>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="9" t="s">
+      <c r="A50" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B50" s="15"/>
-      <c r="C50" s="15"/>
+      <c r="B50" s="14"/>
+      <c r="C50" s="14"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
+      <c r="A51" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B51" s="11"/>
-      <c r="C51" s="11"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
+      <c r="A52" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B52" s="11"/>
-      <c r="C52" s="11"/>
+      <c r="B52" s="10"/>
+      <c r="C52" s="10"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
+      <c r="A53" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B53" s="11"/>
-      <c r="C53" s="11"/>
+      <c r="B53" s="10"/>
+      <c r="C53" s="10"/>
     </row>
     <row r="54" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="7" t="s">
+      <c r="A54" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B54" s="11"/>
-      <c r="C54" s="11"/>
+      <c r="B54" s="10"/>
+      <c r="C54" s="10"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
+      <c r="A55" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B55" s="11"/>
-      <c r="C55" s="11"/>
+      <c r="B55" s="10"/>
+      <c r="C55" s="10"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="10" t="s">
+      <c r="A56" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B56" s="15"/>
-      <c r="C56" s="15"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="14"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="10" t="s">
+      <c r="A57" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B57" s="15">
+      <c r="B57" s="14">
         <f>SUM(B49,B56)</f>
         <v>0</v>
       </c>
-      <c r="C57" s="15">
+      <c r="C57" s="14">
         <f>SUM(C49,C56)</f>
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="9" t="s">
+      <c r="A58" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B58" s="20"/>
-      <c r="C58" s="20"/>
+      <c r="B58" s="19"/>
+      <c r="C58" s="19"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="7" t="s">
+      <c r="A59" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B59" s="13">
+      <c r="B59" s="12">
         <f>SUM(B60:B65)</f>
         <v>0</v>
       </c>
-      <c r="C59" s="13">
+      <c r="C59" s="12">
         <f>SUM(C60:C65)</f>
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="6" t="s">
+      <c r="A60" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B60" s="14"/>
-      <c r="C60" s="14"/>
+      <c r="B60" s="13"/>
+      <c r="C60" s="13"/>
     </row>
     <row r="61" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A61" s="6" t="s">
+      <c r="A61" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B61" s="14"/>
-      <c r="C61" s="14"/>
+      <c r="B61" s="13"/>
+      <c r="C61" s="13"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="6" t="s">
+      <c r="A62" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B62" s="14"/>
-      <c r="C62" s="14"/>
+      <c r="B62" s="13"/>
+      <c r="C62" s="13"/>
     </row>
     <row r="63" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="6" t="s">
+      <c r="A63" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B63" s="14"/>
-      <c r="C63" s="14"/>
+      <c r="B63" s="13"/>
+      <c r="C63" s="13"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="6" t="s">
+      <c r="A64" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B64" s="14"/>
-      <c r="C64" s="14"/>
+      <c r="B64" s="13"/>
+      <c r="C64" s="13"/>
     </row>
     <row r="65" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A65" s="6" t="s">
+      <c r="A65" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B65" s="12"/>
-      <c r="C65" s="12"/>
+      <c r="B65" s="11"/>
+      <c r="C65" s="11"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="9" t="s">
+      <c r="A66" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B66" s="15">
+      <c r="B66" s="14">
         <f>B59</f>
         <v>0</v>
       </c>
-      <c r="C66" s="15">
+      <c r="C66" s="14">
         <f>C59</f>
         <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="7" t="s">
+      <c r="A67" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B67" s="11">
+      <c r="B67" s="10">
         <f>SUM(B68:B70)</f>
         <v>0</v>
       </c>
-      <c r="C67" s="11">
+      <c r="C67" s="10">
         <f>SUM(C68:C70)</f>
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="6" t="s">
+      <c r="A68" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B68" s="12"/>
-      <c r="C68" s="12"/>
+      <c r="B68" s="11"/>
+      <c r="C68" s="11"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="6" t="s">
+      <c r="A69" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B69" s="12"/>
-      <c r="C69" s="12"/>
+      <c r="B69" s="11"/>
+      <c r="C69" s="11"/>
     </row>
     <row r="70" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="6" t="s">
+      <c r="A70" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B70" s="12"/>
-      <c r="C70" s="12"/>
+      <c r="B70" s="11"/>
+      <c r="C70" s="11"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="9" t="s">
+      <c r="A71" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B71" s="15">
+      <c r="B71" s="14">
         <f>B67</f>
         <v>0</v>
       </c>
-      <c r="C71" s="15">
+      <c r="C71" s="14">
         <f>C67</f>
         <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="9" t="s">
+      <c r="A72" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B72" s="15">
+      <c r="B72" s="14">
         <f>SUM(B57,B58,B66,B71)</f>
         <v>0</v>
       </c>
-      <c r="C72" s="15">
+      <c r="C72" s="14">
         <f>SUM(C57,C58,C66,C71)</f>
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="9" t="s">
+      <c r="A73" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B73" s="10"/>
-      <c r="C73" s="10"/>
+      <c r="B73" s="9"/>
+      <c r="C73" s="9"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="10" t="s">
+      <c r="A74" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B74" s="21">
+      <c r="B74" s="20">
         <f>SUM(B72:B73)</f>
         <v>0</v>
       </c>
-      <c r="C74" s="21">
+      <c r="C74" s="20">
         <f>SUM(C72:C73)</f>
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A75" s="16" t="s">
+      <c r="A75" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="B75" s="16"/>
-      <c r="C75" s="16"/>
+      <c r="B75" s="15"/>
+      <c r="C75" s="15"/>
     </row>
     <row r="76" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A76" s="16" t="s">
+      <c r="A76" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="B76" s="16"/>
-      <c r="C76" s="16"/>
+      <c r="B76" s="15"/>
+      <c r="C76" s="15"/>
     </row>
     <row r="77" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A77" s="16" t="s">
+      <c r="A77" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="B77" s="16"/>
-      <c r="C77" s="16"/>
+      <c r="B77" s="15"/>
+      <c r="C77" s="15"/>
     </row>
     <row r="78" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A78" s="18" t="s">
+      <c r="A78" s="17" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A79" s="18" t="s">
+      <c r="A79" s="17" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="22" t="s">
+      <c r="A82" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="B82" s="23"/>
-      <c r="C82" s="24"/>
+      <c r="B82" s="28"/>
+      <c r="C82" s="29"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="2"/>
-      <c r="B84" s="2" t="s">
+      <c r="A84" s="1"/>
+      <c r="B84" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="C84" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="7" t="s">
+      <c r="A85" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B85" s="13">
+      <c r="B85" s="12">
         <f>SUM(B86:B87)</f>
         <v>0</v>
       </c>
-      <c r="C85" s="13">
+      <c r="C85" s="12">
         <f>SUM(C86:C87)</f>
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="6" t="s">
+      <c r="A86" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B86" s="14"/>
-      <c r="C86" s="14"/>
+      <c r="B86" s="13"/>
+      <c r="C86" s="13"/>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="6" t="s">
+      <c r="A87" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B87" s="14"/>
-      <c r="C87" s="14"/>
+      <c r="B87" s="13"/>
+      <c r="C87" s="13"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="9" t="s">
+      <c r="A88" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B88" s="20">
+      <c r="B88" s="19">
         <f>B85</f>
         <v>0</v>
       </c>
-      <c r="C88" s="20">
+      <c r="C88" s="19">
         <f>C85</f>
         <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A89" s="9" t="s">
+      <c r="A89" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B89" s="20"/>
-      <c r="C89" s="20"/>
+      <c r="B89" s="19"/>
+      <c r="C89" s="19"/>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="7" t="s">
+      <c r="A90" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B90" s="13"/>
-      <c r="C90" s="13"/>
+      <c r="B90" s="12"/>
+      <c r="C90" s="12"/>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="7" t="s">
+      <c r="A91" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B91" s="13"/>
-      <c r="C91" s="13"/>
+      <c r="B91" s="12"/>
+      <c r="C91" s="12"/>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="7" t="s">
+      <c r="A92" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B92" s="13"/>
-      <c r="C92" s="13"/>
+      <c r="B92" s="12"/>
+      <c r="C92" s="12"/>
     </row>
     <row r="93" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A93" s="7" t="s">
+      <c r="A93" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B93" s="13"/>
-      <c r="C93" s="13"/>
+      <c r="B93" s="12"/>
+      <c r="C93" s="12"/>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="7" t="s">
+      <c r="A94" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B94" s="13"/>
-      <c r="C94" s="13"/>
+      <c r="B94" s="12"/>
+      <c r="C94" s="12"/>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="9" t="s">
+      <c r="A95" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B95" s="20">
+      <c r="B95" s="19">
         <f>SUM(B90:B94,B85)</f>
         <v>0</v>
       </c>
-      <c r="C95" s="20">
+      <c r="C95" s="19">
         <f>SUM(C90:C94,C85)</f>
         <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="7" t="s">
+      <c r="A96" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B96" s="13">
+      <c r="B96" s="12">
         <f>SUM(B97,B99,B101:B104)</f>
         <v>0</v>
       </c>
-      <c r="C96" s="13">
+      <c r="C96" s="12">
         <f>SUM(C97,C99,C101:C104)</f>
         <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="6" t="s">
+      <c r="A97" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B97" s="14"/>
-      <c r="C97" s="14"/>
+      <c r="B97" s="13"/>
+      <c r="C97" s="13"/>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="26" t="s">
+      <c r="A98" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="B98" s="27"/>
-      <c r="C98" s="27"/>
+      <c r="B98" s="23"/>
+      <c r="C98" s="23"/>
     </row>
     <row r="99" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A99" s="6" t="s">
+      <c r="A99" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B99" s="14"/>
-      <c r="C99" s="14"/>
+      <c r="B99" s="13"/>
+      <c r="C99" s="13"/>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="26" t="s">
+      <c r="A100" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="B100" s="27"/>
-      <c r="C100" s="27"/>
+      <c r="B100" s="23"/>
+      <c r="C100" s="23"/>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="6" t="s">
+      <c r="A101" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B101" s="14"/>
-      <c r="C101" s="14"/>
+      <c r="B101" s="13"/>
+      <c r="C101" s="13"/>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="6" t="s">
+      <c r="A102" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B102" s="14"/>
-      <c r="C102" s="14"/>
+      <c r="B102" s="13"/>
+      <c r="C102" s="13"/>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" s="6" t="s">
+      <c r="A103" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B103" s="14"/>
-      <c r="C103" s="14"/>
+      <c r="B103" s="13"/>
+      <c r="C103" s="13"/>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" s="6" t="s">
+      <c r="A104" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B104" s="14"/>
-      <c r="C104" s="14"/>
+      <c r="B104" s="13"/>
+      <c r="C104" s="13"/>
     </row>
     <row r="105" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A105" s="7" t="s">
+      <c r="A105" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B105" s="13">
+      <c r="B105" s="12">
         <f>SUM(B106:B108)</f>
         <v>0</v>
       </c>
-      <c r="C105" s="13">
+      <c r="C105" s="12">
         <f>SUM(C106:C108)</f>
         <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A106" s="6" t="s">
+      <c r="A106" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B106" s="14"/>
-      <c r="C106" s="14"/>
+      <c r="B106" s="13"/>
+      <c r="C106" s="13"/>
     </row>
     <row r="107" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A107" s="6" t="s">
+      <c r="A107" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B107" s="14"/>
-      <c r="C107" s="14"/>
+      <c r="B107" s="13"/>
+      <c r="C107" s="13"/>
     </row>
     <row r="108" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A108" s="6" t="s">
+      <c r="A108" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B108" s="14"/>
-      <c r="C108" s="14"/>
+      <c r="B108" s="13"/>
+      <c r="C108" s="13"/>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" s="7" t="s">
+      <c r="A109" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B109" s="13"/>
-      <c r="C109" s="13"/>
+      <c r="B109" s="12"/>
+      <c r="C109" s="12"/>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" s="7" t="s">
+      <c r="A110" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B110" s="13"/>
-      <c r="C110" s="13"/>
+      <c r="B110" s="12"/>
+      <c r="C110" s="12"/>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" s="9" t="s">
+      <c r="A111" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="B111" s="20">
+      <c r="B111" s="19">
         <f>SUM(B109:B110,B105,B96)</f>
         <v>0</v>
       </c>
-      <c r="C111" s="20">
+      <c r="C111" s="19">
         <f>SUM(C109:C110,C105,C96)</f>
         <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A112" s="16" t="s">
+      <c r="A112" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="B112" s="25"/>
-      <c r="C112" s="25"/>
+      <c r="B112" s="21"/>
+      <c r="C112" s="21"/>
     </row>
     <row r="113" spans="1:3" ht="87" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="28" t="s">
+      <c r="A113" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="B113" s="29"/>
-      <c r="C113" s="30"/>
+      <c r="B113" s="31"/>
+      <c r="C113" s="32"/>
     </row>
     <row r="114" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="28" t="s">
+      <c r="A114" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="B114" s="29"/>
-      <c r="C114" s="30"/>
+      <c r="B114" s="31"/>
+      <c r="C114" s="32"/>
     </row>
     <row r="115" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A115" s="18" t="s">
+      <c r="A115" s="17" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A116" s="18" t="s">
+      <c r="A116" s="17" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117" s="18" t="s">
+      <c r="A117" s="17" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A118" s="18" t="s">
+      <c r="A118" s="17" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A119" s="18" t="s">
+      <c r="A119" s="17" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="2"/>
-      <c r="B121" s="2" t="s">
+      <c r="A121" s="1"/>
+      <c r="B121" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C121" s="2" t="s">
+      <c r="C121" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="9" t="s">
+      <c r="A122" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="B122" s="20">
+      <c r="B122" s="19">
         <f>B95-B111</f>
         <v>0</v>
       </c>
-      <c r="C122" s="20">
+      <c r="C122" s="19">
         <f>C95-C111</f>
         <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A123" s="9" t="s">
+      <c r="A123" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="B123" s="20"/>
-      <c r="C123" s="20"/>
+      <c r="B123" s="19"/>
+      <c r="C123" s="19"/>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="9" t="s">
+      <c r="A124" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="B124" s="20"/>
-      <c r="C124" s="20"/>
+      <c r="B124" s="19"/>
+      <c r="C124" s="19"/>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" s="9" t="s">
+      <c r="A125" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B125" s="20"/>
-      <c r="C125" s="20"/>
+      <c r="B125" s="19"/>
+      <c r="C125" s="19"/>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="7" t="s">
+      <c r="A126" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B126" s="13">
+      <c r="B126" s="12">
         <f>SUM(B127:B132)</f>
         <v>0</v>
       </c>
-      <c r="C126" s="13">
+      <c r="C126" s="12">
         <f>SUM(C127:C132)</f>
         <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="6" t="s">
+      <c r="A127" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B127" s="14"/>
-      <c r="C127" s="14"/>
+      <c r="B127" s="13"/>
+      <c r="C127" s="13"/>
     </row>
     <row r="128" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A128" s="6" t="s">
+      <c r="A128" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B128" s="14"/>
-      <c r="C128" s="14"/>
+      <c r="B128" s="13"/>
+      <c r="C128" s="13"/>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A129" s="6" t="s">
+      <c r="A129" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B129" s="14"/>
-      <c r="C129" s="14"/>
+      <c r="B129" s="13"/>
+      <c r="C129" s="13"/>
     </row>
     <row r="130" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A130" s="6" t="s">
+      <c r="A130" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B130" s="14"/>
-      <c r="C130" s="14"/>
+      <c r="B130" s="13"/>
+      <c r="C130" s="13"/>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" s="6" t="s">
+      <c r="A131" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B131" s="14"/>
-      <c r="C131" s="14"/>
+      <c r="B131" s="13"/>
+      <c r="C131" s="13"/>
     </row>
     <row r="132" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A132" s="6" t="s">
+      <c r="A132" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B132" s="14"/>
-      <c r="C132" s="14"/>
+      <c r="B132" s="13"/>
+      <c r="C132" s="13"/>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133" s="9" t="s">
+      <c r="A133" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="B133" s="20">
+      <c r="B133" s="19">
         <f>B126</f>
         <v>0</v>
       </c>
-      <c r="C133" s="20">
+      <c r="C133" s="19">
         <f>C126</f>
         <v>0</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A134" s="7" t="s">
+      <c r="A134" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B134" s="13">
+      <c r="B134" s="12">
         <f>SUM(B135:B138)</f>
         <v>0</v>
       </c>
-      <c r="C134" s="13">
+      <c r="C134" s="12">
         <f>SUM(C135:C138)</f>
         <v>0</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A135" s="6" t="s">
+      <c r="A135" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B135" s="14"/>
-      <c r="C135" s="14"/>
+      <c r="B135" s="13"/>
+      <c r="C135" s="13"/>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A136" s="6" t="s">
+      <c r="A136" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B136" s="14"/>
-      <c r="C136" s="14"/>
+      <c r="B136" s="13"/>
+      <c r="C136" s="13"/>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A137" s="6" t="s">
+      <c r="A137" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B137" s="14"/>
-      <c r="C137" s="14"/>
+      <c r="B137" s="13"/>
+      <c r="C137" s="13"/>
     </row>
     <row r="138" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A138" s="6" t="s">
+      <c r="A138" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B138" s="14"/>
-      <c r="C138" s="14"/>
+      <c r="B138" s="13"/>
+      <c r="C138" s="13"/>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139" s="9" t="s">
+      <c r="A139" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="B139" s="20">
+      <c r="B139" s="19">
         <f>B134</f>
         <v>0</v>
       </c>
-      <c r="C139" s="20">
+      <c r="C139" s="19">
         <f>C134</f>
         <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A140" s="9" t="s">
+      <c r="A140" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="B140" s="20">
+      <c r="B140" s="19">
         <f>B133-B139</f>
         <v>0</v>
       </c>
-      <c r="C140" s="20">
+      <c r="C140" s="19">
         <f>C133-C139</f>
         <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A141" s="9" t="s">
+      <c r="A141" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="B141" s="20">
+      <c r="B141" s="19">
         <f>B95-B111+B124-B125+B133-B139</f>
         <v>0</v>
       </c>
-      <c r="C141" s="20">
+      <c r="C141" s="19">
         <f>C95-C111+C124-C125+C133-C139</f>
         <v>0</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A142" s="7" t="s">
+      <c r="A142" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B142" s="13">
+      <c r="B142" s="12">
         <f>SUM(B143:B145)</f>
         <v>0</v>
       </c>
-      <c r="C142" s="13">
+      <c r="C142" s="12">
         <f>SUM(C143:C145)</f>
         <v>0</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A143" s="6" t="s">
+      <c r="A143" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B143" s="14"/>
-      <c r="C143" s="14"/>
+      <c r="B143" s="13"/>
+      <c r="C143" s="13"/>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A144" s="6" t="s">
+      <c r="A144" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B144" s="14"/>
-      <c r="C144" s="14"/>
+      <c r="B144" s="13"/>
+      <c r="C144" s="13"/>
     </row>
     <row r="145" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A145" s="6" t="s">
+      <c r="A145" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B145" s="14"/>
-      <c r="C145" s="14"/>
+      <c r="B145" s="13"/>
+      <c r="C145" s="13"/>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A146" s="9" t="s">
+      <c r="A146" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="B146" s="20">
+      <c r="B146" s="19">
         <f>B142</f>
         <v>0</v>
       </c>
-      <c r="C146" s="20">
+      <c r="C146" s="19">
         <f>C142</f>
         <v>0</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A147" s="7" t="s">
+      <c r="A147" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B147" s="13">
+      <c r="B147" s="12">
         <f>SUM(B148:B150)</f>
         <v>0</v>
       </c>
-      <c r="C147" s="13">
+      <c r="C147" s="12">
         <f>SUM(C148:C150)</f>
         <v>0</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A148" s="6" t="s">
+      <c r="A148" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B148" s="14"/>
-      <c r="C148" s="14"/>
+      <c r="B148" s="13"/>
+      <c r="C148" s="13"/>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A149" s="6" t="s">
+      <c r="A149" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B149" s="14"/>
-      <c r="C149" s="14"/>
+      <c r="B149" s="13"/>
+      <c r="C149" s="13"/>
     </row>
     <row r="150" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A150" s="6" t="s">
+      <c r="A150" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B150" s="14"/>
-      <c r="C150" s="14"/>
+      <c r="B150" s="13"/>
+      <c r="C150" s="13"/>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A151" s="9" t="s">
+      <c r="A151" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="B151" s="20">
+      <c r="B151" s="19">
         <f>B147</f>
         <v>0</v>
       </c>
-      <c r="C151" s="20">
+      <c r="C151" s="19">
         <f>C147</f>
         <v>0</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A152" s="9" t="s">
+      <c r="A152" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="B152" s="20">
+      <c r="B152" s="19">
         <f>B146-B151</f>
         <v>0</v>
       </c>
-      <c r="C152" s="20">
+      <c r="C152" s="19">
         <f>C146-C151</f>
         <v>0</v>
       </c>
     </row>
     <row r="153" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A153" s="9" t="s">
+      <c r="A153" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="B153" s="20"/>
-      <c r="C153" s="20"/>
+      <c r="B153" s="19"/>
+      <c r="C153" s="19"/>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A154" s="9" t="s">
+      <c r="A154" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="B154" s="20"/>
-      <c r="C154" s="20"/>
+      <c r="B154" s="19"/>
+      <c r="C154" s="19"/>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A155" s="9" t="s">
+      <c r="A155" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="B155" s="20">
+      <c r="B155" s="19">
         <f>B95+B124+B133+B146</f>
         <v>0</v>
       </c>
-      <c r="C155" s="20">
+      <c r="C155" s="19">
         <f>C95+C124+C133+C146</f>
         <v>0</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A156" s="9" t="s">
+      <c r="A156" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="B156" s="20">
+      <c r="B156" s="19">
         <f>B111+B125+B139+B151+B153+B154</f>
         <v>0</v>
       </c>
-      <c r="C156" s="20">
+      <c r="C156" s="19">
         <f>C111+C125+C139+C151+C153+C154</f>
         <v>0</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A157" s="9" t="s">
+      <c r="A157" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="B157" s="20">
+      <c r="B157" s="19">
         <f>B141+B152+B153+B154</f>
         <v>0</v>
       </c>
-      <c r="C157" s="20">
+      <c r="C157" s="19">
         <f>C141+C152+C153+C154</f>
         <v>0</v>
       </c>
     </row>
     <row r="158" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A158" s="16" t="s">
+      <c r="A158" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="B158" s="25"/>
-      <c r="C158" s="25"/>
+      <c r="B158" s="21"/>
+      <c r="C158" s="21"/>
     </row>
     <row r="159" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A159" s="16" t="s">
+      <c r="A159" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="B159" s="25"/>
-      <c r="C159" s="25"/>
+      <c r="B159" s="21"/>
+      <c r="C159" s="21"/>
     </row>
     <row r="160" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A160" s="31" t="s">
+      <c r="A160" s="24" t="s">
         <v>113</v>
       </c>
     </row>
@@ -2245,12 +2404,525 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="35"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" s="12">
+        <f>SUM(B5,B7,B9:B17)</f>
+        <v>0</v>
+      </c>
+      <c r="C4" s="12">
+        <f>SUM(C5,C7,C9:C17)</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" s="12">
+        <f>SUM(E5:E10,E17)</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="12">
+        <f>SUM(F5:F10,F17)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+    </row>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="19">
+        <f>B4</f>
+        <v>0</v>
+      </c>
+      <c r="C18" s="19">
+        <f>C4</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E18" s="19">
+        <f>E4</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="19">
+        <f>F4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="25"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+    </row>
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B22" s="19">
+        <f>SUM(B20:B21,B18)</f>
+        <v>0</v>
+      </c>
+      <c r="C22" s="19">
+        <f>SUM(C20:C21,C18)</f>
+        <v>0</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="E22" s="19">
+        <f>SUM(E20,E18)</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="19">
+        <f>SUM(F20,F18)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="19">
+        <f>SUM(B22:B23)</f>
+        <v>0</v>
+      </c>
+      <c r="C24" s="19">
+        <f>SUM(C22:C23)</f>
+        <v>0</v>
+      </c>
+      <c r="D24" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="41">
+        <f>SUM(E22:E23)</f>
+        <v>0</v>
+      </c>
+      <c r="F24" s="41">
+        <f>SUM(F22:F23)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="42"/>
+    </row>
+    <row r="26" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="38"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
+    </row>
+    <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+    </row>
+    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+    </row>
+    <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="B30" s="37"/>
+      <c r="C30" s="37"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="37"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="37"/>
+      <c r="B31" s="37"/>
+      <c r="C31" s="37"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="37"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="37"/>
+      <c r="B32" s="37"/>
+      <c r="C32" s="37"/>
+      <c r="D32" s="37"/>
+      <c r="E32" s="37"/>
+      <c r="F32" s="37"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="37"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="37"/>
+      <c r="D33" s="37"/>
+      <c r="E33" s="37"/>
+      <c r="F33" s="37"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="37"/>
+      <c r="B34" s="37"/>
+      <c r="C34" s="37"/>
+      <c r="D34" s="37"/>
+      <c r="E34" s="37"/>
+      <c r="F34" s="37"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="37"/>
+      <c r="B35" s="37"/>
+      <c r="C35" s="37"/>
+      <c r="D35" s="37"/>
+      <c r="E35" s="37"/>
+      <c r="F35" s="37"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="37"/>
+      <c r="B36" s="37"/>
+      <c r="C36" s="37"/>
+      <c r="D36" s="37"/>
+      <c r="E36" s="37"/>
+      <c r="F36" s="37"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="37"/>
+      <c r="B37" s="37"/>
+      <c r="C37" s="37"/>
+      <c r="D37" s="37"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="37"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="37"/>
+      <c r="B38" s="37"/>
+      <c r="C38" s="37"/>
+      <c r="D38" s="37"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="37"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="37"/>
+      <c r="B39" s="37"/>
+      <c r="C39" s="37"/>
+      <c r="D39" s="37"/>
+      <c r="E39" s="37"/>
+      <c r="F39" s="37"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="37"/>
+      <c r="B40" s="37"/>
+      <c r="C40" s="37"/>
+      <c r="D40" s="37"/>
+      <c r="E40" s="37"/>
+      <c r="F40" s="37"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="7"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="7"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="7"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="7"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="7"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F24:F25"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Compte de resultat en liste _ Systeme abrege
</commit_message>
<xml_diff>
--- a/France/3_Comptabilite_Et_Fiscalite/2_Compte_De_Resultat/Compte_De_Resultat.xlsx
+++ b/France/3_Comptabilite_Et_Fiscalite/2_Compte_De_Resultat/Compte_De_Resultat.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Systeme_De_Base" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="165">
   <si>
     <t xml:space="preserve"> Modèle de compte de résultat en tableau</t>
   </si>
@@ -472,6 +472,70 @@
   </si>
   <si>
     <t>Solde débiteur : perte (3)</t>
+  </si>
+  <si>
+    <t>Modèle de compte de résultat en liste</t>
+  </si>
+  <si>
+    <t>Produits d’exploitation (hors taxes) :</t>
+  </si>
+  <si>
+    <t>Subventions d’exploitation</t>
+  </si>
+  <si>
+    <t>Total (I) dont à l’exportation</t>
+  </si>
+  <si>
+    <t>Charges d’exploitation (hors taxes) :</t>
+  </si>
+  <si>
+    <t>Achats de marchandises ('c')</t>
+  </si>
+  <si>
+    <t>Variation de stock (marchandises) (d)</t>
+  </si>
+  <si>
+    <t>Achats d’approvisionnements ('c')</t>
+  </si>
+  <si>
+    <t>Variation de stock d’approvisionnements (d)</t>
+  </si>
+  <si>
+    <t>Autres charges externes *</t>
+  </si>
+  <si>
+    <t>RESULTAT D'EXPLOITATION (I - II)</t>
+  </si>
+  <si>
+    <t>Produits financiers (1) (III)</t>
+  </si>
+  <si>
+    <t>Charges financières (IV)</t>
+  </si>
+  <si>
+    <t>Produits exceptionnels (1) (V)</t>
+  </si>
+  <si>
+    <t>Charges exceptionnelles (VI)</t>
+  </si>
+  <si>
+    <t>Impôts sur les bénéfices (VII)</t>
+  </si>
+  <si>
+    <t>BENEFICE ou PERTE (I - II + III - IV + V - VI - VII) (2)</t>
+  </si>
+  <si>
+    <t>* Y compris :
+- redevances de crédit-bail mobilier
+- redevances de crédit-bail immobilier
+(1) Dont reprises sur dépréciations, provisions (et amortissements)
+(2) Compte tenu d'un résultat exceptionnel de (V - VI) ou (VI - V)</t>
+  </si>
+  <si>
+    <t>(b) Stock final moins stock initial.</t>
+  </si>
+  <si>
+    <t>(d) Stock initial moins stock final.</t>
   </si>
 </sst>
 </file>
@@ -644,7 +708,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -770,6 +834,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="6" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2404,10 +2486,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2813,9 +2895,11 @@
       <c r="F32" s="37"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="37"/>
-      <c r="B33" s="37"/>
-      <c r="C33" s="37"/>
+      <c r="A33" s="43" t="s">
+        <v>145</v>
+      </c>
+      <c r="B33" s="44"/>
+      <c r="C33" s="45"/>
       <c r="D33" s="37"/>
       <c r="E33" s="37"/>
       <c r="F33" s="37"/>
@@ -2829,99 +2913,391 @@
       <c r="F34" s="37"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="37"/>
-      <c r="B35" s="37"/>
-      <c r="C35" s="37"/>
+      <c r="A35" s="1"/>
+      <c r="B35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="D35" s="37"/>
       <c r="E35" s="37"/>
       <c r="F35" s="37"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="37"/>
-      <c r="B36" s="37"/>
-      <c r="C36" s="37"/>
+      <c r="A36" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B36" s="12">
+        <f>SUM(B37:B42)</f>
+        <v>0</v>
+      </c>
+      <c r="C36" s="12">
+        <f>SUM(C37:C42)</f>
+        <v>0</v>
+      </c>
       <c r="D36" s="37"/>
       <c r="E36" s="37"/>
       <c r="F36" s="37"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="37"/>
-      <c r="B37" s="37"/>
-      <c r="C37" s="37"/>
+      <c r="A37" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
       <c r="D37" s="37"/>
       <c r="E37" s="37"/>
       <c r="F37" s="37"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="37"/>
-      <c r="B38" s="37"/>
-      <c r="C38" s="37"/>
+      <c r="A38" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
       <c r="D38" s="37"/>
       <c r="E38" s="37"/>
       <c r="F38" s="37"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="37"/>
-      <c r="B39" s="37"/>
-      <c r="C39" s="37"/>
+      <c r="A39" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
       <c r="D39" s="37"/>
       <c r="E39" s="37"/>
       <c r="F39" s="37"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="37"/>
-      <c r="B40" s="37"/>
-      <c r="C40" s="37"/>
+      <c r="A40" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
       <c r="D40" s="37"/>
       <c r="E40" s="37"/>
       <c r="F40" s="37"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="7"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
+      <c r="A41" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13"/>
       <c r="D41" s="7"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="7"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
+      <c r="A42" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42" s="13"/>
+      <c r="C42" s="13"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="7"/>
-      <c r="B43" s="7"/>
-      <c r="C43" s="7"/>
+      <c r="A43" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B43" s="19">
+        <f>B36</f>
+        <v>0</v>
+      </c>
+      <c r="C43" s="19">
+        <f>C36</f>
+        <v>0</v>
+      </c>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="7"/>
-      <c r="B44" s="7"/>
-      <c r="C44" s="7"/>
+      <c r="A44" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="B44" s="19"/>
+      <c r="C44" s="19"/>
       <c r="D44" s="7"/>
       <c r="E44" s="7"/>
       <c r="F44" s="7"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="7"/>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7"/>
+      <c r="A45" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B45" s="12">
+        <f>SUM(B46,B48,B50:B57)</f>
+        <v>0</v>
+      </c>
+      <c r="C45" s="12">
+        <f>SUM(C46,C48,C50:C57)</f>
+        <v>0</v>
+      </c>
       <c r="D45" s="7"/>
       <c r="E45" s="7"/>
       <c r="F45" s="7"/>
     </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B46" s="13"/>
+      <c r="C46" s="13"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="B47" s="23"/>
+      <c r="C47" s="23"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B48" s="13"/>
+      <c r="C48" s="13"/>
+    </row>
+    <row r="49" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="B49" s="23"/>
+      <c r="C49" s="23"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B50" s="13"/>
+      <c r="C50" s="13"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B51" s="13"/>
+      <c r="C51" s="13"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B52" s="13"/>
+      <c r="C52" s="13"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B53" s="13"/>
+      <c r="C53" s="13"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B54" s="13"/>
+      <c r="C54" s="13"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B55" s="13"/>
+      <c r="C55" s="13"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B56" s="13"/>
+      <c r="C56" s="13"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B57" s="13"/>
+      <c r="C57" s="13"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B58" s="19">
+        <f>B45</f>
+        <v>0</v>
+      </c>
+      <c r="C58" s="19">
+        <f>C45</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B59" s="19">
+        <f>B43-B58</f>
+        <v>0</v>
+      </c>
+      <c r="C59" s="19">
+        <f>C43-C58</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="B60" s="19"/>
+      <c r="C60" s="19"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B61" s="19"/>
+      <c r="C61" s="19"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="B62" s="19"/>
+      <c r="C62" s="19"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B63" s="19"/>
+      <c r="C63" s="19"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="B64" s="19"/>
+      <c r="C64" s="19"/>
+    </row>
+    <row r="65" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="B65" s="19">
+        <f>B43-B58+B60-B61+B62-B63-B64</f>
+        <v>0</v>
+      </c>
+      <c r="C65" s="19">
+        <f>C43-C58+C60-C61+C62-C63-C64</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="48" t="s">
+        <v>162</v>
+      </c>
+      <c r="B66" s="48"/>
+      <c r="C66" s="48"/>
+    </row>
+    <row r="67" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B67" s="46"/>
+      <c r="C67" s="46"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="B68" s="46"/>
+      <c r="C68" s="46"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="B69" s="46"/>
+      <c r="C69" s="46"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="B70" s="46"/>
+      <c r="C70" s="46"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="47"/>
+      <c r="B71" s="46"/>
+      <c r="C71" s="46"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="47"/>
+      <c r="B72" s="46"/>
+      <c r="C72" s="46"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="47"/>
+      <c r="B73" s="46"/>
+      <c r="C73" s="46"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="47"/>
+      <c r="B74" s="46"/>
+      <c r="C74" s="46"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="47"/>
+      <c r="B75" s="46"/>
+      <c r="C75" s="46"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="47"/>
+      <c r="B76" s="46"/>
+      <c r="C76" s="46"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="47"/>
+      <c r="B77" s="46"/>
+      <c r="C77" s="46"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="47"/>
+      <c r="B78" s="46"/>
+      <c r="C78" s="46"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="47"/>
+      <c r="B79" s="46"/>
+      <c r="C79" s="46"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="47"/>
+      <c r="B80" s="46"/>
+      <c r="C80" s="46"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="47"/>
+      <c r="B81" s="46"/>
+      <c r="C81" s="46"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="A66:C66"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="D24:D25"/>
     <mergeCell ref="E24:E25"/>
     <mergeCell ref="F24:F25"/>
+    <mergeCell ref="A33:C33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2931,7 +3307,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
Compte de résultat _ Systeme developpe
</commit_message>
<xml_diff>
--- a/France/3_Comptabilite_Et_Fiscalite/2_Compte_De_Resultat/Compte_De_Resultat.xlsx
+++ b/France/3_Comptabilite_Et_Fiscalite/2_Compte_De_Resultat/Compte_De_Resultat.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="229">
   <si>
     <t xml:space="preserve"> Modèle de compte de résultat en tableau</t>
   </si>
@@ -536,6 +536,206 @@
   </si>
   <si>
     <t>(d) Stock initial moins stock final.</t>
+  </si>
+  <si>
+    <t>Modèle de compte de résultat</t>
+  </si>
+  <si>
+    <t>Totaux partiels</t>
+  </si>
+  <si>
+    <t>Totaux
+partiels</t>
+  </si>
+  <si>
+    <t>Coût d'achat des marchandises vendues dans l'exercice</t>
+  </si>
+  <si>
+    <t>(-) Achats de marchandises (a)</t>
+  </si>
+  <si>
+    <t>(-) Variation des stocks de marchandises (b)</t>
+  </si>
+  <si>
+    <t>Consommations de l'exercice en provenance de tiers</t>
+  </si>
+  <si>
+    <t>(-) Achats stockés d'approvisionnements (a) :</t>
+  </si>
+  <si>
+    <t>(--) matières premières</t>
+  </si>
+  <si>
+    <t>(--) autres approvisionnements</t>
+  </si>
+  <si>
+    <t>(-) Variation des stocks d'approvisionnements (b)</t>
+  </si>
+  <si>
+    <t>(-) Achats de sous-traitances</t>
+  </si>
+  <si>
+    <t>(-) Achats non stockés de matières et fournitures</t>
+  </si>
+  <si>
+    <t>(-) Services extérieurs :</t>
+  </si>
+  <si>
+    <t>(--) personnel extérieur</t>
+  </si>
+  <si>
+    <t>(--) loyers en crédit-bail (c)</t>
+  </si>
+  <si>
+    <t>(--) autres</t>
+  </si>
+  <si>
+    <t>Sur rémunérations</t>
+  </si>
+  <si>
+    <t>Autres</t>
+  </si>
+  <si>
+    <t>Charges de personnel</t>
+  </si>
+  <si>
+    <t>Dotations aux amortissements et dépréciations</t>
+  </si>
+  <si>
+    <t>Sur immobilisations : dotations aux amortissements (d)</t>
+  </si>
+  <si>
+    <t>Quote-parts de résultat sur opérations faites en commun</t>
+  </si>
+  <si>
+    <t>Charges nettes sur cessions de VMP</t>
+  </si>
+  <si>
+    <t>Charges exceptionnelles</t>
+  </si>
+  <si>
+    <t>Sur opérations en capital :</t>
+  </si>
+  <si>
+    <t>(-) valeurs comptables des éléments immobilisés et financiers cédés ('e')</t>
+  </si>
+  <si>
+    <t>(-) autres</t>
+  </si>
+  <si>
+    <t>Dotations aux amortissements, aux dépréciations et aux provisions :</t>
+  </si>
+  <si>
+    <t>(-) dotations aux provisions réglementées</t>
+  </si>
+  <si>
+    <t>(-) dotations aux amortissements, aux dépréciations et aux autres provisions</t>
+  </si>
+  <si>
+    <t>Participation des salariés aux résultats</t>
+  </si>
+  <si>
+    <t>Impôts sur les bénéfices</t>
+  </si>
+  <si>
+    <t>Solde créditeur = bénéfice</t>
+  </si>
+  <si>
+    <t>(1) Dont charges afférentes à des exercices antérieurs.
+Les conséquences des corrections d’erreurs significatives, calculées après impôt, sont
+présentées sur une ligne séparée sauf s’il s’agit de corriger une écriture ayant été
+directement imputée sur les capitaux propres.</t>
+  </si>
+  <si>
+    <t>(2) Dont intérêts concernant les entités liées.</t>
+  </si>
+  <si>
+    <t>(a) Y compris frais accessoires.</t>
+  </si>
+  <si>
+    <t>(c) A ventiler en "mobilier" et "immobilier".</t>
+  </si>
+  <si>
+    <t>(d) Y compris éventuellement dotations aux amortissements des charges à répartir.</t>
+  </si>
+  <si>
+    <t>(e) A l'exception des valeurs mobilières de placement.</t>
+  </si>
+  <si>
+    <t>Production vendue</t>
+  </si>
+  <si>
+    <t>Ventes</t>
+  </si>
+  <si>
+    <t>Travaux</t>
+  </si>
+  <si>
+    <t>Prestations de services</t>
+  </si>
+  <si>
+    <t>dont à l'exportation : ........</t>
+  </si>
+  <si>
+    <t>Production stockée (a)</t>
+  </si>
+  <si>
+    <t>En-cours de production de biens (a)</t>
+  </si>
+  <si>
+    <t>En-cours de production de services (a)</t>
+  </si>
+  <si>
+    <t>Produits (a)</t>
+  </si>
+  <si>
+    <t>Reprises sur provisions, dépréciations (et amortissements)</t>
+  </si>
+  <si>
+    <t>Transferts de charges</t>
+  </si>
+  <si>
+    <t>Quote-part de résultat sur opérations faites en commun</t>
+  </si>
+  <si>
+    <t>Produits financiers</t>
+  </si>
+  <si>
+    <t>D'autres valeurs mobilières de créances de l'actif immobilisé (2)</t>
+  </si>
+  <si>
+    <t>Reprises sur provisions et dépréciations et transfert de charges financières</t>
+  </si>
+  <si>
+    <t>Produits exceptionnels</t>
+  </si>
+  <si>
+    <t>(-) produits des cessions d'éléments d'actif (c)</t>
+  </si>
+  <si>
+    <t>(-) subventions d'investissement virées au résultat de l'exercice</t>
+  </si>
+  <si>
+    <t>Reprises sur provisions et dépréciations et transferts de charges exceptionnelles</t>
+  </si>
+  <si>
+    <t>Solde débiteur = perte</t>
+  </si>
+  <si>
+    <t>(1) Dont produits afférents à des exercices antérieurs.
+Les conséquences des corrections d’erreurs significatives, calculées après impôt, sont
+présentées sur une ligne séparée sauf s’il s’agit de corriger une écriture ayant été directement
+imputée sur les capitaux propres.</t>
+  </si>
+  <si>
+    <t>(2) Dont produits concernant les entités liées</t>
+  </si>
+  <si>
+    <t>(a) Stock final moins stock initial : montant de la variation en moins entre parenthèses ou précédé du signe (-)
+dans le cas de déstockage de production.</t>
+  </si>
+  <si>
+    <t>(c) A l'exception des valeurs mobilières de placement.</t>
   </si>
 </sst>
 </file>
@@ -545,7 +745,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -560,8 +760,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -613,6 +819,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -708,7 +920,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -785,6 +997,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -806,6 +1051,9 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -815,15 +1063,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -845,15 +1084,29 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="2" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Monétaire" xfId="1" builtinId="4"/>
@@ -1173,11 +1426,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
+      <c r="A1" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
@@ -1817,11 +2070,11 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="27" t="s">
+      <c r="A82" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="B82" s="28"/>
-      <c r="C82" s="29"/>
+      <c r="B82" s="39"/>
+      <c r="C82" s="40"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
@@ -2065,18 +2318,18 @@
       <c r="C112" s="21"/>
     </row>
     <row r="113" spans="1:3" ht="87" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="30" t="s">
+      <c r="A113" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="B113" s="31"/>
-      <c r="C113" s="32"/>
+      <c r="B113" s="42"/>
+      <c r="C113" s="43"/>
     </row>
     <row r="114" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="30" t="s">
+      <c r="A114" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="B114" s="31"/>
-      <c r="C114" s="32"/>
+      <c r="B114" s="42"/>
+      <c r="C114" s="43"/>
     </row>
     <row r="115" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A115" s="17" t="s">
@@ -2503,14 +2756,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="45" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="35"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="47"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -2635,8 +2888,8 @@
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
       <c r="D11" s="25"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
@@ -2645,8 +2898,8 @@
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
       <c r="D12" s="25"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -2655,8 +2908,8 @@
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
       <c r="D13" s="25"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
@@ -2665,8 +2918,8 @@
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
       <c r="D14" s="25"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
@@ -2675,8 +2928,8 @@
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
       <c r="D15" s="25"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
@@ -2685,8 +2938,8 @@
       <c r="B16" s="13"/>
       <c r="C16" s="13"/>
       <c r="D16" s="25"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
@@ -2726,8 +2979,8 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="25"/>
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
       <c r="D19" s="8" t="s">
         <v>141</v>
       </c>
@@ -2753,8 +3006,8 @@
       <c r="B21" s="19"/>
       <c r="C21" s="19"/>
       <c r="D21" s="25"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
@@ -2804,14 +3057,14 @@
         <f>SUM(C22:C23)</f>
         <v>0</v>
       </c>
-      <c r="D24" s="39" t="s">
+      <c r="D24" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="E24" s="41">
+      <c r="E24" s="50">
         <f>SUM(E22:E23)</f>
         <v>0</v>
       </c>
-      <c r="F24" s="41">
+      <c r="F24" s="50">
         <f>SUM(F22:F23)</f>
         <v>0</v>
       </c>
@@ -2822,9 +3075,9 @@
       </c>
       <c r="B25" s="21"/>
       <c r="C25" s="21"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="42"/>
-      <c r="F25" s="42"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="51"/>
+      <c r="F25" s="51"/>
     </row>
     <row r="26" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
@@ -2842,7 +3095,7 @@
       <c r="A27" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B27" s="38"/>
+      <c r="B27" s="28"/>
       <c r="C27" s="25"/>
       <c r="D27" s="25"/>
       <c r="E27" s="25"/>
@@ -2852,65 +3105,65 @@
       <c r="A28" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
     </row>
     <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
     </row>
     <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="B30" s="37"/>
-      <c r="C30" s="37"/>
-      <c r="D30" s="37"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="37"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="37"/>
-      <c r="B31" s="37"/>
-      <c r="C31" s="37"/>
-      <c r="D31" s="37"/>
-      <c r="E31" s="37"/>
-      <c r="F31" s="37"/>
+      <c r="A31" s="27"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="37"/>
-      <c r="B32" s="37"/>
-      <c r="C32" s="37"/>
-      <c r="D32" s="37"/>
-      <c r="E32" s="37"/>
-      <c r="F32" s="37"/>
+      <c r="A32" s="27"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="43" t="s">
+      <c r="A33" s="52" t="s">
         <v>145</v>
       </c>
-      <c r="B33" s="44"/>
-      <c r="C33" s="45"/>
-      <c r="D33" s="37"/>
-      <c r="E33" s="37"/>
-      <c r="F33" s="37"/>
+      <c r="B33" s="53"/>
+      <c r="C33" s="54"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="27"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="37"/>
-      <c r="B34" s="37"/>
-      <c r="C34" s="37"/>
-      <c r="D34" s="37"/>
-      <c r="E34" s="37"/>
-      <c r="F34" s="37"/>
+      <c r="A34" s="27"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
@@ -2920,9 +3173,9 @@
       <c r="C35" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D35" s="37"/>
-      <c r="E35" s="37"/>
-      <c r="F35" s="37"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
@@ -2936,9 +3189,9 @@
         <f>SUM(C37:C42)</f>
         <v>0</v>
       </c>
-      <c r="D36" s="37"/>
-      <c r="E36" s="37"/>
-      <c r="F36" s="37"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
@@ -2946,9 +3199,9 @@
       </c>
       <c r="B37" s="13"/>
       <c r="C37" s="13"/>
-      <c r="D37" s="37"/>
-      <c r="E37" s="37"/>
-      <c r="F37" s="37"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
@@ -2956,9 +3209,9 @@
       </c>
       <c r="B38" s="13"/>
       <c r="C38" s="13"/>
-      <c r="D38" s="37"/>
-      <c r="E38" s="37"/>
-      <c r="F38" s="37"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="27"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
@@ -2966,9 +3219,9 @@
       </c>
       <c r="B39" s="13"/>
       <c r="C39" s="13"/>
-      <c r="D39" s="37"/>
-      <c r="E39" s="37"/>
-      <c r="F39" s="37"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="27"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
@@ -2976,9 +3229,9 @@
       </c>
       <c r="B40" s="13"/>
       <c r="C40" s="13"/>
-      <c r="D40" s="37"/>
-      <c r="E40" s="37"/>
-      <c r="F40" s="37"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
@@ -3201,94 +3454,94 @@
       </c>
     </row>
     <row r="66" spans="1:3" ht="81" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="48" t="s">
+      <c r="A66" s="44" t="s">
         <v>162</v>
       </c>
-      <c r="B66" s="48"/>
-      <c r="C66" s="48"/>
+      <c r="B66" s="44"/>
+      <c r="C66" s="44"/>
     </row>
     <row r="67" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="B67" s="46"/>
-      <c r="C67" s="46"/>
+      <c r="B67" s="29"/>
+      <c r="C67" s="29"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="B68" s="46"/>
-      <c r="C68" s="46"/>
+      <c r="B68" s="29"/>
+      <c r="C68" s="29"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="B69" s="46"/>
-      <c r="C69" s="46"/>
+      <c r="B69" s="29"/>
+      <c r="C69" s="29"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="B70" s="46"/>
-      <c r="C70" s="46"/>
+      <c r="B70" s="29"/>
+      <c r="C70" s="29"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="47"/>
-      <c r="B71" s="46"/>
-      <c r="C71" s="46"/>
+      <c r="A71" s="30"/>
+      <c r="B71" s="29"/>
+      <c r="C71" s="29"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="47"/>
-      <c r="B72" s="46"/>
-      <c r="C72" s="46"/>
+      <c r="A72" s="30"/>
+      <c r="B72" s="29"/>
+      <c r="C72" s="29"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="47"/>
-      <c r="B73" s="46"/>
-      <c r="C73" s="46"/>
+      <c r="A73" s="30"/>
+      <c r="B73" s="29"/>
+      <c r="C73" s="29"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="47"/>
-      <c r="B74" s="46"/>
-      <c r="C74" s="46"/>
+      <c r="A74" s="30"/>
+      <c r="B74" s="29"/>
+      <c r="C74" s="29"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="47"/>
-      <c r="B75" s="46"/>
-      <c r="C75" s="46"/>
+      <c r="A75" s="30"/>
+      <c r="B75" s="29"/>
+      <c r="C75" s="29"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="47"/>
-      <c r="B76" s="46"/>
-      <c r="C76" s="46"/>
+      <c r="A76" s="30"/>
+      <c r="B76" s="29"/>
+      <c r="C76" s="29"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="47"/>
-      <c r="B77" s="46"/>
-      <c r="C77" s="46"/>
+      <c r="A77" s="30"/>
+      <c r="B77" s="29"/>
+      <c r="C77" s="29"/>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="47"/>
-      <c r="B78" s="46"/>
-      <c r="C78" s="46"/>
+      <c r="A78" s="30"/>
+      <c r="B78" s="29"/>
+      <c r="C78" s="29"/>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="47"/>
-      <c r="B79" s="46"/>
-      <c r="C79" s="46"/>
+      <c r="A79" s="30"/>
+      <c r="B79" s="29"/>
+      <c r="C79" s="29"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="47"/>
-      <c r="B80" s="46"/>
-      <c r="C80" s="46"/>
+      <c r="A80" s="30"/>
+      <c r="B80" s="29"/>
+      <c r="C80" s="29"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="47"/>
-      <c r="B81" s="46"/>
-      <c r="C81" s="46"/>
+      <c r="A81" s="30"/>
+      <c r="B81" s="29"/>
+      <c r="C81" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -3305,12 +3558,870 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="F100" sqref="F100"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="45" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="47"/>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="55"/>
+      <c r="D3" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="33"/>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="55"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32" t="s">
+        <v>166</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="E4" s="34"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12">
+        <f>SUM(C6,C9,C20,C23,C26,C31:C33)</f>
+        <v>0</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="E5" s="27"/>
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13">
+        <f>SUM(B7:B8)</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="27"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="27"/>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
+        <v>170</v>
+      </c>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="27"/>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13">
+        <f>SUM(B10,B13:B16)</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="13"/>
+      <c r="E9" s="27"/>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="B10" s="23">
+        <f>SUM(B11:B12)</f>
+        <v>0</v>
+      </c>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="27"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="35" t="s">
+        <v>173</v>
+      </c>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="27"/>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="35" t="s">
+        <v>174</v>
+      </c>
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="27"/>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="27"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="27"/>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="27"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="B16" s="23">
+        <f>SUM(B17:B19)</f>
+        <v>0</v>
+      </c>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="27"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="35" t="s">
+        <v>179</v>
+      </c>
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="27"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="35" t="s">
+        <v>180</v>
+      </c>
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="27"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="35" t="s">
+        <v>181</v>
+      </c>
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="27"/>
+    </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13">
+        <f>SUM(B21:B22)</f>
+        <v>0</v>
+      </c>
+      <c r="D20" s="13"/>
+      <c r="E20" s="27"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="B21" s="23"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="27"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="27"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11">
+        <f>SUM(B24:B25)</f>
+        <v>0</v>
+      </c>
+      <c r="D23" s="11"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="56" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="58"/>
+      <c r="C24" s="58"/>
+      <c r="D24" s="58"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="58"/>
+      <c r="C25" s="58"/>
+      <c r="D25" s="58"/>
+    </row>
+    <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11">
+        <f>SUM(B27:B30)</f>
+        <v>0</v>
+      </c>
+      <c r="D26" s="11"/>
+    </row>
+    <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="B27" s="58"/>
+      <c r="C27" s="58"/>
+      <c r="D27" s="58"/>
+    </row>
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" s="58"/>
+      <c r="C28" s="58"/>
+      <c r="D28" s="58"/>
+    </row>
+    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="58"/>
+      <c r="C29" s="58"/>
+      <c r="D29" s="58"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="58"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="58"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+    </row>
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11">
+        <f>SUM(B34:B37)</f>
+        <v>0</v>
+      </c>
+      <c r="D33" s="11"/>
+    </row>
+    <row r="34" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A34" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34" s="58"/>
+      <c r="C34" s="58"/>
+      <c r="D34" s="58"/>
+    </row>
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" s="58"/>
+      <c r="C35" s="58"/>
+      <c r="D35" s="58"/>
+    </row>
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" s="58"/>
+      <c r="C36" s="58"/>
+      <c r="D36" s="58"/>
+    </row>
+    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="22" t="s">
+        <v>188</v>
+      </c>
+      <c r="B37" s="58"/>
+      <c r="C37" s="58"/>
+      <c r="D37" s="58"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="B38" s="63"/>
+      <c r="C38" s="63">
+        <f>SUM(B39:B40,B43)</f>
+        <v>0</v>
+      </c>
+      <c r="D38" s="63"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="57" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" s="64"/>
+      <c r="C39" s="64"/>
+      <c r="D39" s="64"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B40" s="64">
+        <f>SUM(B41:B42)</f>
+        <v>0</v>
+      </c>
+      <c r="C40" s="64"/>
+      <c r="D40" s="64"/>
+    </row>
+    <row r="41" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="22" t="s">
+        <v>191</v>
+      </c>
+      <c r="B41" s="58"/>
+      <c r="C41" s="58"/>
+      <c r="D41" s="58"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="56" t="s">
+        <v>192</v>
+      </c>
+      <c r="B42" s="58"/>
+      <c r="C42" s="58"/>
+      <c r="D42" s="58"/>
+    </row>
+    <row r="43" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A43" s="57" t="s">
+        <v>193</v>
+      </c>
+      <c r="B43" s="64">
+        <f>SUM(B44:B45)</f>
+        <v>0</v>
+      </c>
+      <c r="C43" s="64"/>
+      <c r="D43" s="64"/>
+    </row>
+    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="60" t="s">
+        <v>194</v>
+      </c>
+      <c r="B44" s="65"/>
+      <c r="C44" s="65"/>
+      <c r="D44" s="65"/>
+    </row>
+    <row r="45" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A45" s="60" t="s">
+        <v>195</v>
+      </c>
+      <c r="B45" s="65"/>
+      <c r="C45" s="65"/>
+      <c r="D45" s="65"/>
+    </row>
+    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="61" t="s">
+        <v>196</v>
+      </c>
+      <c r="B46" s="63"/>
+      <c r="C46" s="63"/>
+      <c r="D46" s="63"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B47" s="10"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B48" s="10"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="10"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B49" s="14"/>
+      <c r="C49" s="14">
+        <f>SUM(C46:C48,C38,C5)</f>
+        <v>0</v>
+      </c>
+      <c r="D49" s="14">
+        <f>SUM(D46:D48,D38,D5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="44" t="s">
+        <v>199</v>
+      </c>
+      <c r="B50" s="44"/>
+      <c r="C50" s="62"/>
+      <c r="D50" s="62"/>
+    </row>
+    <row r="51" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="44" t="s">
+        <v>200</v>
+      </c>
+      <c r="B51" s="44"/>
+      <c r="C51" s="62"/>
+      <c r="D51" s="62"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="17" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A53" s="17" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="17" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A55" s="17" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="17" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="55" t="s">
+        <v>42</v>
+      </c>
+      <c r="B58" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="C58" s="55"/>
+      <c r="D58" s="32" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="55"/>
+      <c r="B59" s="32"/>
+      <c r="C59" s="32" t="s">
+        <v>166</v>
+      </c>
+      <c r="D59" s="32" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B60" s="12"/>
+      <c r="C60" s="12">
+        <f>SUM(C61:C62,C68,C72:C78,C85,C92)</f>
+        <v>0</v>
+      </c>
+      <c r="D60" s="12">
+        <f>SUM(D61:D62,D68,D72:D78,D85,D92)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B61" s="13"/>
+      <c r="C61" s="13"/>
+      <c r="D61" s="13"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B62" s="13"/>
+      <c r="C62" s="13">
+        <f>SUM(B63:B65)</f>
+        <v>0</v>
+      </c>
+      <c r="D62" s="13"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="B63" s="23"/>
+      <c r="C63" s="23"/>
+      <c r="D63" s="23"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="22" t="s">
+        <v>207</v>
+      </c>
+      <c r="B64" s="23"/>
+      <c r="C64" s="23"/>
+      <c r="D64" s="23"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="B65" s="23"/>
+      <c r="C65" s="23"/>
+      <c r="D65" s="23"/>
+    </row>
+    <row r="66" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A66" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B66" s="19"/>
+      <c r="C66" s="19"/>
+      <c r="D66" s="19"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="B67" s="19"/>
+      <c r="C67" s="19"/>
+      <c r="D67" s="19"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="B68" s="13"/>
+      <c r="C68" s="13">
+        <f>SUM(B69:B71)</f>
+        <v>0</v>
+      </c>
+      <c r="D68" s="13"/>
+    </row>
+    <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="B69" s="23"/>
+      <c r="C69" s="23"/>
+      <c r="D69" s="23"/>
+    </row>
+    <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="B70" s="23"/>
+      <c r="C70" s="23"/>
+      <c r="D70" s="23"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="22" t="s">
+        <v>213</v>
+      </c>
+      <c r="B71" s="23"/>
+      <c r="C71" s="23"/>
+      <c r="D71" s="23"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B72" s="13"/>
+      <c r="C72" s="13"/>
+      <c r="D72" s="13"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B73" s="13"/>
+      <c r="C73" s="13"/>
+      <c r="D73" s="13"/>
+    </row>
+    <row r="74" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A74" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="B74" s="13"/>
+      <c r="C74" s="13"/>
+      <c r="D74" s="13"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="B75" s="13"/>
+      <c r="C75" s="13"/>
+      <c r="D75" s="13"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B76" s="13"/>
+      <c r="C76" s="13"/>
+      <c r="D76" s="13"/>
+    </row>
+    <row r="77" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A77" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="B77" s="13"/>
+      <c r="C77" s="13"/>
+      <c r="D77" s="13"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B78" s="64"/>
+      <c r="C78" s="64">
+        <f>SUM(B79:B84)</f>
+        <v>0</v>
+      </c>
+      <c r="D78" s="64"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="B79" s="59"/>
+      <c r="C79" s="59"/>
+      <c r="D79" s="59"/>
+    </row>
+    <row r="80" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A80" s="22" t="s">
+        <v>218</v>
+      </c>
+      <c r="B80" s="59"/>
+      <c r="C80" s="59"/>
+      <c r="D80" s="59"/>
+    </row>
+    <row r="81" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A81" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B81" s="23"/>
+      <c r="C81" s="23"/>
+      <c r="D81" s="23"/>
+    </row>
+    <row r="82" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A82" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="B82" s="23"/>
+      <c r="C82" s="23"/>
+      <c r="D82" s="23"/>
+    </row>
+    <row r="83" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A83" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B83" s="23"/>
+      <c r="C83" s="23"/>
+      <c r="D83" s="23"/>
+    </row>
+    <row r="84" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A84" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B84" s="23"/>
+      <c r="C84" s="23"/>
+      <c r="D84" s="23"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="B85" s="13"/>
+      <c r="C85" s="13">
+        <f>SUM(B86:B87,B91)</f>
+        <v>0</v>
+      </c>
+      <c r="D85" s="13"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B86" s="23"/>
+      <c r="C86" s="23"/>
+      <c r="D86" s="23"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="B87" s="23"/>
+      <c r="C87" s="23"/>
+      <c r="D87" s="23"/>
+    </row>
+    <row r="88" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A88" s="35" t="s">
+        <v>221</v>
+      </c>
+      <c r="B88" s="36"/>
+      <c r="C88" s="36"/>
+      <c r="D88" s="36"/>
+    </row>
+    <row r="89" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A89" s="35" t="s">
+        <v>222</v>
+      </c>
+      <c r="B89" s="36"/>
+      <c r="C89" s="36"/>
+      <c r="D89" s="36"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="35" t="s">
+        <v>192</v>
+      </c>
+      <c r="B90" s="36"/>
+      <c r="C90" s="36"/>
+      <c r="D90" s="36"/>
+    </row>
+    <row r="91" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A91" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="B91" s="23"/>
+      <c r="C91" s="23"/>
+      <c r="D91" s="23"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="B92" s="13"/>
+      <c r="C92" s="13"/>
+      <c r="D92" s="13"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B93" s="19"/>
+      <c r="C93" s="19">
+        <f>C60</f>
+        <v>0</v>
+      </c>
+      <c r="D93" s="19">
+        <f>D60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="41" t="s">
+        <v>225</v>
+      </c>
+      <c r="B94" s="43"/>
+      <c r="C94" s="31"/>
+      <c r="D94" s="31"/>
+    </row>
+    <row r="95" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="41" t="s">
+        <v>226</v>
+      </c>
+      <c r="B95" s="43"/>
+      <c r="C95" s="31"/>
+      <c r="D95" s="31"/>
+    </row>
+    <row r="96" spans="1:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="17" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A97" s="17" t="s">
+        <v>228</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>